<commit_message>
Preprocessing Skenario Modul 3
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ricky\Informatika\7Smester7\Pembelajaran Mesin\TugasPraktikumML-18_247-18_249\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392DE55E-7D1D-4405-B1FB-8AD0860C1A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA3772F-E0A7-48A7-AD58-7BBBB196E2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -412,25 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -438,6 +420,24 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,21 +657,21 @@
   <dimension ref="A1:Z1015"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" style="14" customWidth="1"/>
-    <col min="27" max="16384" width="14.42578125" style="14"/>
+    <col min="1" max="1" width="9.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" style="11" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -704,25 +704,25 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="16" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="1"/>
@@ -746,12 +746,12 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="17"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -990,15 +990,21 @@
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="3">
+        <v>44508</v>
+      </c>
       <c r="E9" s="3">
         <v>44510</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="3">
+        <v>44509</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1171,7 +1177,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="19"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
         <v>15</v>
@@ -1205,7 +1211,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="19"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
         <v>15</v>
@@ -1239,7 +1245,7 @@
         <v>11</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="19"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
         <v>15</v>
@@ -1273,7 +1279,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="19"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
         <v>15</v>
@@ -1307,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="19"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
         <v>15</v>
@@ -1341,7 +1347,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6" t="s">
         <v>15</v>
@@ -1375,7 +1381,7 @@
         <v>8</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="19"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6" t="s">
         <v>15</v>
@@ -1409,7 +1415,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="19"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
         <v>15</v>
@@ -1443,7 +1449,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="19"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6" t="s">
         <v>15</v>
@@ -1477,7 +1483,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="19"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6" t="s">
         <v>15</v>
@@ -1504,10 +1510,10 @@
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="18"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="19"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="7"/>

</xml_diff>

<commit_message>
update sprint_project lalu push pakai colab
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Modelling CNN - Skenario Praktikum Modul 4 - Skema 1</t>
-  </si>
-  <si>
-    <t>ON GOING</t>
   </si>
   <si>
     <t>Model Evaluation - Skenario Praktikum Modul 4 - Skema 1</t>
@@ -341,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -383,6 +380,9 @@
     </xf>
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1164,7 +1164,9 @@
       <c r="G14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1192,15 +1194,21 @@
       <c r="C15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="13">
+        <v>44532.0</v>
+      </c>
       <c r="E15" s="14">
         <v>44533.0</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16" t="s">
-        <v>25</v>
+      <c r="F15" s="14">
+        <v>44533.0</v>
       </c>
-      <c r="H15" s="12"/>
+      <c r="G15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1223,20 +1231,26 @@
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="13">
+        <v>44532.0</v>
+      </c>
       <c r="E16" s="14">
         <v>44533.0</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16" t="s">
-        <v>25</v>
+      <c r="F16" s="14">
+        <v>44533.0</v>
       </c>
-      <c r="H16" s="12"/>
+      <c r="G16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1259,20 +1273,26 @@
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="13">
+        <v>44532.0</v>
+      </c>
       <c r="E17" s="14">
         <v>44533.0</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16" t="s">
-        <v>25</v>
+      <c r="F17" s="14">
+        <v>44533.0</v>
       </c>
-      <c r="H17" s="12"/>
+      <c r="G17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1295,20 +1315,26 @@
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="13">
+        <v>44532.0</v>
+      </c>
       <c r="E18" s="14">
         <v>44533.0</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16" t="s">
-        <v>25</v>
+      <c r="F18" s="14">
+        <v>44533.0</v>
       </c>
-      <c r="H18" s="12"/>
+      <c r="G18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1331,16 +1357,16 @@
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16" t="s">
-        <v>30</v>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="1"/>
@@ -1365,16 +1391,16 @@
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16" t="s">
-        <v>30</v>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="1"/>
@@ -1399,16 +1425,16 @@
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="16"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16" t="s">
-        <v>30</v>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="1"/>
@@ -1433,16 +1459,16 @@
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16" t="s">
-        <v>30</v>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="1"/>
@@ -1467,16 +1493,16 @@
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="16"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16" t="s">
-        <v>30</v>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="1"/>
@@ -1500,12 +1526,12 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
       <c r="H24" s="12"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1528,13 +1554,13 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="20"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>

</xml_diff>